<commit_message>
Update Closed zones list
</commit_message>
<xml_diff>
--- a/data/var/ktes.xlsx
+++ b/data/var/ktes.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\kte\src\misc\closed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My\Repo\kte\data\var\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="z" sheetId="1" r:id="rId1"/>
+    <sheet name="2023-03-13" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>FILE</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
 </sst>
 </file>
@@ -1022,9 +1034,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1687,6 +1701,80 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="5">
+        <v>8</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>